<commit_message>
Nové vstupy, nové tabulky, přidány Excelové výstupy
</commit_message>
<xml_diff>
--- a/vystupy/tabulky/operacni-programy-zamestnanci.xlsx
+++ b/vystupy/tabulky/operacni-programy-zamestnanci.xlsx
@@ -596,7 +596,7 @@
         <v>2.82</v>
       </c>
       <c r="M2" t="n">
-        <v>115.11</v>
+        <v>110.92</v>
       </c>
       <c r="N2" t="n">
         <v>464.06</v>
@@ -605,18 +605,18 @@
         <v>5.17</v>
       </c>
       <c r="P2" t="n">
-        <v>1111.02</v>
+        <v>997.15</v>
       </c>
       <c r="Q2" t="s"/>
       <c r="R2" t="s"/>
       <c r="S2" t="n">
-        <v>329.66</v>
+        <v>426.93</v>
       </c>
       <c r="T2" t="n">
         <v>44.77</v>
       </c>
       <c r="U2" t="n">
-        <v>446.9</v>
+        <v>395.79</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -624,55 +624,55 @@
         <v>22</v>
       </c>
       <c r="B3" t="n">
-        <v>16.1</v>
+        <v>16.18</v>
       </c>
       <c r="C3" t="n">
         <v>42.5</v>
       </c>
       <c r="D3" t="n">
-        <v>9.35</v>
+        <v>9.42</v>
       </c>
       <c r="E3" t="n">
-        <v>9.85</v>
+        <v>9.890000000000001</v>
       </c>
       <c r="F3" t="n">
-        <v>11.28</v>
+        <v>11.37</v>
       </c>
       <c r="G3" t="n">
-        <v>7.89</v>
+        <v>7.94</v>
       </c>
       <c r="H3" t="n">
-        <v>9.34</v>
+        <v>9.369999999999999</v>
       </c>
       <c r="I3" t="n">
-        <v>10.37</v>
+        <v>10.41</v>
       </c>
       <c r="J3" t="n">
-        <v>12.07</v>
+        <v>12.17</v>
       </c>
       <c r="K3" t="n">
-        <v>14.43</v>
+        <v>14.48</v>
       </c>
       <c r="L3" t="n">
-        <v>29.72</v>
+        <v>29.75</v>
       </c>
       <c r="M3" t="n">
-        <v>23.01</v>
+        <v>23.03</v>
       </c>
       <c r="N3" t="n">
-        <v>25.12</v>
+        <v>25.23</v>
       </c>
       <c r="O3" t="n">
         <v>65.7</v>
       </c>
       <c r="P3" t="n">
-        <v>20.35</v>
+        <v>20.37</v>
       </c>
       <c r="Q3" t="n">
         <v>53.72</v>
       </c>
       <c r="R3" t="n">
-        <v>40.59</v>
+        <v>40.61</v>
       </c>
       <c r="S3" t="n">
         <v>9.82</v>
@@ -695,7 +695,7 @@
         <v>23.38</v>
       </c>
       <c r="D4" t="n">
-        <v>42.6</v>
+        <v>42.5</v>
       </c>
       <c r="E4" t="n">
         <v>110.83</v>
@@ -710,19 +710,19 @@
         <v>45.28</v>
       </c>
       <c r="I4" t="n">
-        <v>12.74</v>
+        <v>12.71</v>
       </c>
       <c r="J4" t="n">
-        <v>28.22</v>
+        <v>28.23</v>
       </c>
       <c r="K4" t="n">
-        <v>536.04</v>
+        <v>536.03</v>
       </c>
       <c r="L4" t="n">
         <v>24.88</v>
       </c>
       <c r="M4" t="n">
-        <v>72.01000000000001</v>
+        <v>71.95</v>
       </c>
       <c r="N4" t="n">
         <v>32.78</v>
@@ -740,7 +740,7 @@
         <v>63.4</v>
       </c>
       <c r="S4" t="n">
-        <v>60.02</v>
+        <v>59.96</v>
       </c>
       <c r="T4" t="n">
         <v>68.37</v>
@@ -760,13 +760,13 @@
         <v>3.24</v>
       </c>
       <c r="D5" t="n">
-        <v>8.380000000000001</v>
+        <v>8.390000000000001</v>
       </c>
       <c r="E5" t="n">
         <v>6.97</v>
       </c>
       <c r="F5" t="n">
-        <v>9.029999999999999</v>
+        <v>9.02</v>
       </c>
       <c r="G5" t="n">
         <v>5.56</v>
@@ -787,7 +787,7 @@
         <v>16.67</v>
       </c>
       <c r="M5" t="n">
-        <v>34.48</v>
+        <v>34.57</v>
       </c>
       <c r="N5" t="n">
         <v>24.5</v>
@@ -855,7 +855,7 @@
         <v>167.98</v>
       </c>
       <c r="R6" t="n">
-        <v>243.79</v>
+        <v>249.04</v>
       </c>
       <c r="S6" t="s"/>
       <c r="T6" t="n">
@@ -892,19 +892,19 @@
         <v>20.52</v>
       </c>
       <c r="J7" t="n">
-        <v>22.36</v>
+        <v>22.38</v>
       </c>
       <c r="K7" t="n">
         <v>8.83</v>
       </c>
       <c r="L7" t="n">
-        <v>11.88</v>
+        <v>11.79</v>
       </c>
       <c r="M7" t="n">
-        <v>46.63</v>
+        <v>46.55</v>
       </c>
       <c r="N7" t="n">
-        <v>136.12</v>
+        <v>136.07</v>
       </c>
       <c r="O7" t="n">
         <v>38.7</v>
@@ -933,7 +933,7 @@
         <v>27</v>
       </c>
       <c r="B8" t="n">
-        <v>5.09</v>
+        <v>5.1</v>
       </c>
       <c r="C8" t="n">
         <v>2.55</v>
@@ -963,7 +963,7 @@
         <v>16.8</v>
       </c>
       <c r="L8" t="n">
-        <v>25.45</v>
+        <v>25.54</v>
       </c>
       <c r="M8" t="n">
         <v>21.78</v>
@@ -1021,7 +1021,7 @@
         <v>4.81</v>
       </c>
       <c r="K9" t="n">
-        <v>19.61</v>
+        <v>19.59</v>
       </c>
       <c r="L9" t="n">
         <v>18.61</v>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="C10" t="s"/>
       <c r="D10" t="n">
-        <v>27.82</v>
+        <v>27.69</v>
       </c>
       <c r="E10" t="n">
         <v>32.23</v>
@@ -1065,10 +1065,10 @@
         <v>18.37</v>
       </c>
       <c r="H10" t="n">
-        <v>87.95999999999999</v>
+        <v>87.97</v>
       </c>
       <c r="I10" t="n">
-        <v>65.16</v>
+        <v>65.06999999999999</v>
       </c>
       <c r="J10" t="n">
         <v>34.1</v>
@@ -1077,14 +1077,14 @@
         <v>73.73999999999999</v>
       </c>
       <c r="L10" t="n">
-        <v>50.26</v>
+        <v>50.24</v>
       </c>
       <c r="M10" t="n">
-        <v>80.5</v>
+        <v>83.52</v>
       </c>
       <c r="N10" t="s"/>
       <c r="O10" t="n">
-        <v>87.88</v>
+        <v>86.88</v>
       </c>
       <c r="P10" t="s"/>
       <c r="Q10" t="s"/>
@@ -1115,13 +1115,13 @@
         <v>29.02</v>
       </c>
       <c r="G11" t="n">
-        <v>17.08</v>
+        <v>17.29</v>
       </c>
       <c r="H11" t="n">
         <v>15.69</v>
       </c>
       <c r="I11" t="n">
-        <v>28.51</v>
+        <v>28.49</v>
       </c>
       <c r="J11" t="n">
         <v>30.4</v>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="O11" t="s"/>
       <c r="P11" t="n">
-        <v>73.45999999999999</v>
+        <v>71.02</v>
       </c>
       <c r="Q11" t="n">
         <v>59.67</v>
@@ -1151,7 +1151,7 @@
       <c r="S11" t="s"/>
       <c r="T11" t="s"/>
       <c r="U11" t="n">
-        <v>158.36</v>
+        <v>191.95</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1216,7 +1216,7 @@
         <v>32</v>
       </c>
       <c r="B13" t="n">
-        <v>21.06</v>
+        <v>21</v>
       </c>
       <c r="C13" t="n">
         <v>2.42</v>
@@ -1228,7 +1228,7 @@
         <v>18.64</v>
       </c>
       <c r="F13" t="n">
-        <v>24.48</v>
+        <v>24.25</v>
       </c>
       <c r="G13" t="n">
         <v>21.41</v>
@@ -1249,10 +1249,10 @@
         <v>42.1</v>
       </c>
       <c r="M13" t="n">
-        <v>78.12</v>
+        <v>78.09999999999999</v>
       </c>
       <c r="N13" t="n">
-        <v>46.32</v>
+        <v>46.29</v>
       </c>
       <c r="O13" t="s"/>
       <c r="P13" t="s"/>
@@ -1286,7 +1286,7 @@
         <v>33.59</v>
       </c>
       <c r="G14" t="n">
-        <v>57.95</v>
+        <v>57.93</v>
       </c>
       <c r="H14" t="n">
         <v>42.32</v>
@@ -1301,7 +1301,7 @@
         <v>85.2</v>
       </c>
       <c r="L14" t="n">
-        <v>119.99</v>
+        <v>119.98</v>
       </c>
       <c r="M14" t="n">
         <v>56.12</v>
@@ -1507,7 +1507,7 @@
         <v>8.27</v>
       </c>
       <c r="J18" t="n">
-        <v>16.66</v>
+        <v>16.73</v>
       </c>
       <c r="K18" t="n">
         <v>22.07</v>
@@ -1532,7 +1532,7 @@
         <v>25.17</v>
       </c>
       <c r="S18" t="n">
-        <v>32.5</v>
+        <v>33.29</v>
       </c>
       <c r="T18" t="n">
         <v>35.06</v>
@@ -1597,7 +1597,7 @@
         <v>1.1</v>
       </c>
       <c r="S19" t="n">
-        <v>20.97</v>
+        <v>20.98</v>
       </c>
       <c r="T19" t="n">
         <v>9.890000000000001</v>
@@ -1763,25 +1763,25 @@
       <c r="J2" t="s"/>
       <c r="K2" t="s"/>
       <c r="L2" t="n">
-        <v>77.27</v>
+        <v>73.08</v>
       </c>
       <c r="M2" t="n">
         <v>464.06</v>
       </c>
       <c r="N2" t="s"/>
       <c r="O2" t="n">
-        <v>1111.02</v>
+        <v>997.15</v>
       </c>
       <c r="P2" t="s"/>
       <c r="Q2" t="s"/>
       <c r="R2" t="n">
-        <v>329.66</v>
+        <v>426.93</v>
       </c>
       <c r="S2" t="n">
         <v>44.77</v>
       </c>
       <c r="T2" t="n">
-        <v>446.9</v>
+        <v>395.79</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -1789,52 +1789,52 @@
         <v>22</v>
       </c>
       <c r="B3" t="n">
-        <v>12.69</v>
+        <v>12.76</v>
       </c>
       <c r="C3" t="n">
-        <v>5.28</v>
+        <v>5.33</v>
       </c>
       <c r="D3" t="n">
-        <v>4.49</v>
+        <v>4.54</v>
       </c>
       <c r="E3" t="n">
-        <v>5.56</v>
+        <v>5.61</v>
       </c>
       <c r="F3" t="n">
-        <v>4.91</v>
+        <v>4.95</v>
       </c>
       <c r="G3" t="n">
-        <v>5.89</v>
+        <v>5.92</v>
       </c>
       <c r="H3" t="n">
-        <v>5.47</v>
+        <v>5.5</v>
       </c>
       <c r="I3" t="n">
-        <v>7.6</v>
+        <v>7.7</v>
       </c>
       <c r="J3" t="n">
-        <v>9.93</v>
+        <v>9.970000000000001</v>
       </c>
       <c r="K3" t="n">
-        <v>11.97</v>
+        <v>12</v>
       </c>
       <c r="L3" t="n">
-        <v>7.8</v>
+        <v>7.82</v>
       </c>
       <c r="M3" t="n">
-        <v>11.48</v>
+        <v>11.59</v>
       </c>
       <c r="N3" t="n">
-        <v>17.05</v>
+        <v>17.06</v>
       </c>
       <c r="O3" t="n">
-        <v>15.82</v>
+        <v>15.84</v>
       </c>
       <c r="P3" t="n">
         <v>53.72</v>
       </c>
       <c r="Q3" t="n">
-        <v>8.43</v>
+        <v>8.460000000000001</v>
       </c>
       <c r="R3" t="n">
         <v>9.82</v>
@@ -1923,7 +1923,7 @@
         <v>3.44</v>
       </c>
       <c r="H5" t="n">
-        <v>2.58</v>
+        <v>2.59</v>
       </c>
       <c r="I5" t="n">
         <v>3.62</v>
@@ -1935,7 +1935,7 @@
         <v>13.02</v>
       </c>
       <c r="L5" t="n">
-        <v>30.58</v>
+        <v>30.67</v>
       </c>
       <c r="M5" t="n">
         <v>20.27</v>
@@ -1996,7 +1996,7 @@
         <v>167.98</v>
       </c>
       <c r="Q6" t="n">
-        <v>243.79</v>
+        <v>249.04</v>
       </c>
       <c r="R6" t="s"/>
       <c r="S6" t="n">
@@ -2032,19 +2032,19 @@
         <v>5.35</v>
       </c>
       <c r="I7" t="n">
-        <v>9.970000000000001</v>
+        <v>9.99</v>
       </c>
       <c r="J7" t="n">
         <v>5.49</v>
       </c>
       <c r="K7" t="n">
-        <v>10.25</v>
+        <v>10.16</v>
       </c>
       <c r="L7" t="n">
-        <v>21.31</v>
+        <v>21.23</v>
       </c>
       <c r="M7" t="n">
-        <v>38.37</v>
+        <v>38.32</v>
       </c>
       <c r="N7" t="n">
         <v>38.7</v>
@@ -2100,7 +2100,7 @@
         <v>7.25</v>
       </c>
       <c r="K8" t="n">
-        <v>17.69</v>
+        <v>17.79</v>
       </c>
       <c r="L8" t="n">
         <v>16.4</v>
@@ -2149,7 +2149,7 @@
         <v>4.81</v>
       </c>
       <c r="J9" t="n">
-        <v>19.61</v>
+        <v>19.59</v>
       </c>
       <c r="K9" t="n">
         <v>18.61</v>
@@ -2180,7 +2180,7 @@
         <v>5.89</v>
       </c>
       <c r="C10" t="n">
-        <v>5.22</v>
+        <v>5.08</v>
       </c>
       <c r="D10" t="n">
         <v>12.22</v>
@@ -2195,7 +2195,7 @@
         <v>40.58</v>
       </c>
       <c r="H10" t="n">
-        <v>37.6</v>
+        <v>37.52</v>
       </c>
       <c r="I10" t="n">
         <v>25.02</v>
@@ -2204,14 +2204,14 @@
         <v>33.49</v>
       </c>
       <c r="K10" t="n">
-        <v>39.53</v>
+        <v>39.52</v>
       </c>
       <c r="L10" t="n">
-        <v>65.69</v>
+        <v>68.70999999999999</v>
       </c>
       <c r="M10" t="s"/>
       <c r="N10" t="n">
-        <v>87.88</v>
+        <v>86.88</v>
       </c>
       <c r="O10" t="s"/>
       <c r="P10" t="s"/>
@@ -2241,13 +2241,13 @@
         <v>6.58</v>
       </c>
       <c r="F11" t="n">
-        <v>9.48</v>
+        <v>9.68</v>
       </c>
       <c r="G11" t="n">
         <v>5.12</v>
       </c>
       <c r="H11" t="n">
-        <v>11.63</v>
+        <v>11.62</v>
       </c>
       <c r="I11" t="n">
         <v>16.92</v>
@@ -2266,7 +2266,7 @@
       </c>
       <c r="N11" t="s"/>
       <c r="O11" t="n">
-        <v>73.45999999999999</v>
+        <v>71.02</v>
       </c>
       <c r="P11" t="n">
         <v>59.67</v>
@@ -2277,7 +2277,7 @@
       <c r="R11" t="s"/>
       <c r="S11" t="s"/>
       <c r="T11" t="n">
-        <v>115.86</v>
+        <v>149.45</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -2339,7 +2339,7 @@
         <v>32</v>
       </c>
       <c r="B13" t="n">
-        <v>14.85</v>
+        <v>14.79</v>
       </c>
       <c r="C13" t="n">
         <v>5.95</v>
@@ -2369,10 +2369,10 @@
         <v>22.67</v>
       </c>
       <c r="L13" t="n">
-        <v>32.2</v>
+        <v>32.19</v>
       </c>
       <c r="M13" t="n">
-        <v>11.81</v>
+        <v>11.77</v>
       </c>
       <c r="N13" t="s"/>
       <c r="O13" t="s"/>
@@ -2598,7 +2598,7 @@
         <v>2.9</v>
       </c>
       <c r="I18" t="n">
-        <v>10.8</v>
+        <v>10.87</v>
       </c>
       <c r="J18" t="n">
         <v>18.33</v>
@@ -2623,7 +2623,7 @@
         <v>25.17</v>
       </c>
       <c r="R18" t="n">
-        <v>32.5</v>
+        <v>33.29</v>
       </c>
       <c r="S18" t="n">
         <v>35.06</v>
@@ -2679,7 +2679,7 @@
         <v>1.1</v>
       </c>
       <c r="R19" t="n">
-        <v>19.56</v>
+        <v>19.57</v>
       </c>
       <c r="S19" t="n">
         <v>3.45</v>
@@ -2870,34 +2870,34 @@
         <v>22</v>
       </c>
       <c r="B3" t="n">
-        <v>3.41</v>
+        <v>3.42</v>
       </c>
       <c r="C3" t="n">
         <v>42.5</v>
       </c>
       <c r="D3" t="n">
-        <v>4.07</v>
+        <v>4.09</v>
       </c>
       <c r="E3" t="n">
         <v>5.35</v>
       </c>
       <c r="F3" t="n">
-        <v>5.72</v>
+        <v>5.76</v>
       </c>
       <c r="G3" t="n">
-        <v>2.98</v>
+        <v>2.99</v>
       </c>
       <c r="H3" t="n">
         <v>3.45</v>
       </c>
       <c r="I3" t="n">
-        <v>4.9</v>
+        <v>4.91</v>
       </c>
       <c r="J3" t="n">
         <v>4.47</v>
       </c>
       <c r="K3" t="n">
-        <v>4.5</v>
+        <v>4.51</v>
       </c>
       <c r="L3" t="n">
         <v>17.75</v>
@@ -2935,7 +2935,7 @@
         <v>23.38</v>
       </c>
       <c r="D4" t="n">
-        <v>6.72</v>
+        <v>6.62</v>
       </c>
       <c r="E4" t="n">
         <v>5.71</v>
@@ -2950,19 +2950,19 @@
         <v>5.68</v>
       </c>
       <c r="I4" t="n">
-        <v>5.68</v>
+        <v>5.66</v>
       </c>
       <c r="J4" t="n">
-        <v>6.7</v>
+        <v>6.71</v>
       </c>
       <c r="K4" t="n">
-        <v>8.539999999999999</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="L4" t="n">
         <v>12.56</v>
       </c>
       <c r="M4" t="n">
-        <v>16.74</v>
+        <v>16.68</v>
       </c>
       <c r="N4" t="n">
         <v>28.97</v>
@@ -2980,7 +2980,7 @@
         <v>19.81</v>
       </c>
       <c r="S4" t="n">
-        <v>60.02</v>
+        <v>59.96</v>
       </c>
       <c r="T4" t="n">
         <v>27.24</v>
@@ -3006,7 +3006,7 @@
         <v>3.79</v>
       </c>
       <c r="F5" t="n">
-        <v>3.65</v>
+        <v>3.64</v>
       </c>
       <c r="G5" t="n">
         <v>3.26</v>
@@ -3394,7 +3394,7 @@
         <v>12.47</v>
       </c>
       <c r="F13" t="n">
-        <v>16.11</v>
+        <v>15.89</v>
       </c>
       <c r="G13" t="n">
         <v>12.65</v>
@@ -3446,7 +3446,7 @@
         <v>20.26</v>
       </c>
       <c r="G14" t="n">
-        <v>28.29</v>
+        <v>28.28</v>
       </c>
       <c r="H14" t="n">
         <v>24.74</v>
@@ -3880,18 +3880,18 @@
         <v>4</v>
       </c>
       <c r="P2" t="n">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="Q2" t="s"/>
       <c r="R2" t="s"/>
       <c r="S2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T2" t="n">
         <v>4</v>
       </c>
       <c r="U2" t="n">
-        <v>203</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -3899,7 +3899,7 @@
         <v>22</v>
       </c>
       <c r="B3" t="n">
-        <v>1927</v>
+        <v>1930</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -3911,16 +3911,16 @@
         <v>2377</v>
       </c>
       <c r="F3" t="n">
-        <v>3051</v>
+        <v>3050</v>
       </c>
       <c r="G3" t="n">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="H3" t="n">
         <v>2017</v>
       </c>
       <c r="I3" t="n">
-        <v>1725</v>
+        <v>1726</v>
       </c>
       <c r="J3" t="n">
         <v>1533</v>
@@ -3932,7 +3932,7 @@
         <v>948</v>
       </c>
       <c r="M3" t="n">
-        <v>1030</v>
+        <v>1032</v>
       </c>
       <c r="N3" t="n">
         <v>157</v>
@@ -3985,7 +3985,7 @@
         <v>2259</v>
       </c>
       <c r="I4" t="n">
-        <v>2247</v>
+        <v>2246</v>
       </c>
       <c r="J4" t="n">
         <v>2038</v>
@@ -4029,19 +4029,19 @@
         <v>24</v>
       </c>
       <c r="B5" t="n">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C5" t="n">
         <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="E5" t="n">
         <v>312</v>
       </c>
       <c r="F5" t="n">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G5" t="n">
         <v>179</v>
@@ -4050,7 +4050,7 @@
         <v>490</v>
       </c>
       <c r="I5" t="n">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="J5" t="n">
         <v>659</v>
@@ -4062,7 +4062,7 @@
         <v>558</v>
       </c>
       <c r="M5" t="n">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="N5" t="n">
         <v>128</v>
@@ -4130,7 +4130,7 @@
         <v>24</v>
       </c>
       <c r="R6" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S6" t="s"/>
       <c r="T6" t="n">
@@ -4167,13 +4167,13 @@
         <v>328</v>
       </c>
       <c r="J7" t="n">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="K7" t="n">
         <v>205</v>
       </c>
       <c r="L7" t="n">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="M7" t="n">
         <v>319</v>
@@ -4208,13 +4208,13 @@
         <v>27</v>
       </c>
       <c r="B8" t="n">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C8" t="n">
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="E8" t="n">
         <v>841</v>
@@ -4238,7 +4238,7 @@
         <v>91</v>
       </c>
       <c r="L8" t="n">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M8" t="n">
         <v>216</v>
@@ -4328,7 +4328,7 @@
       </c>
       <c r="C10" t="s"/>
       <c r="D10" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E10" t="n">
         <v>23</v>
@@ -4355,7 +4355,7 @@
         <v>71</v>
       </c>
       <c r="M10" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N10" t="s"/>
       <c r="O10" t="n">
@@ -4396,7 +4396,7 @@
         <v>150</v>
       </c>
       <c r="I11" t="n">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J11" t="n">
         <v>101</v>
@@ -4415,7 +4415,7 @@
       </c>
       <c r="O11" t="s"/>
       <c r="P11" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q11" t="n">
         <v>1</v>
@@ -4503,7 +4503,7 @@
         <v>123</v>
       </c>
       <c r="F13" t="n">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G13" t="n">
         <v>58</v>
@@ -4782,7 +4782,7 @@
         <v>34</v>
       </c>
       <c r="J18" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K18" t="n">
         <v>16</v>
@@ -4807,7 +4807,7 @@
         <v>4</v>
       </c>
       <c r="S18" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T18" t="n">
         <v>10</v>
@@ -5045,18 +5045,18 @@
       </c>
       <c r="N2" t="s"/>
       <c r="O2" t="n">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="P2" t="s"/>
       <c r="Q2" t="s"/>
       <c r="R2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="S2" t="n">
         <v>4</v>
       </c>
       <c r="T2" t="n">
-        <v>203</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -5094,7 +5094,7 @@
         <v>831</v>
       </c>
       <c r="L3" t="n">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="M3" t="n">
         <v>123</v>
@@ -5198,7 +5198,7 @@
         <v>54</v>
       </c>
       <c r="H5" t="n">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I5" t="n">
         <v>247</v>
@@ -5210,7 +5210,7 @@
         <v>246</v>
       </c>
       <c r="L5" t="n">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="M5" t="n">
         <v>62</v>
@@ -5271,7 +5271,7 @@
         <v>24</v>
       </c>
       <c r="Q6" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R6" t="s"/>
       <c r="S6" t="n">
@@ -5307,13 +5307,13 @@
         <v>282</v>
       </c>
       <c r="I7" t="n">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J7" t="n">
         <v>167</v>
       </c>
       <c r="K7" t="n">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="L7" t="n">
         <v>315</v>
@@ -5375,7 +5375,7 @@
         <v>85</v>
       </c>
       <c r="K8" t="n">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L8" t="n">
         <v>215</v>
@@ -5455,7 +5455,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D10" t="n">
         <v>15</v>
@@ -5482,7 +5482,7 @@
         <v>69</v>
       </c>
       <c r="L10" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M10" t="s"/>
       <c r="N10" t="n">
@@ -5522,7 +5522,7 @@
         <v>136</v>
       </c>
       <c r="H11" t="n">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I11" t="n">
         <v>90</v>
@@ -5541,7 +5541,7 @@
       </c>
       <c r="N11" t="s"/>
       <c r="O11" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="P11" t="n">
         <v>1</v>
@@ -5873,7 +5873,7 @@
         <v>4</v>
       </c>
       <c r="I18" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J18" t="n">
         <v>14</v>
@@ -5898,7 +5898,7 @@
         <v>4</v>
       </c>
       <c r="R18" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S18" t="n">
         <v>10</v>
@@ -6145,7 +6145,7 @@
         <v>22</v>
       </c>
       <c r="B3" t="n">
-        <v>1611</v>
+        <v>1614</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -6157,16 +6157,16 @@
         <v>188</v>
       </c>
       <c r="F3" t="n">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G3" t="n">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H3" t="n">
         <v>435</v>
       </c>
       <c r="I3" t="n">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="J3" t="n">
         <v>226</v>
@@ -6225,7 +6225,7 @@
         <v>2254</v>
       </c>
       <c r="I4" t="n">
-        <v>2233</v>
+        <v>2232</v>
       </c>
       <c r="J4" t="n">
         <v>1991</v>
@@ -6269,19 +6269,19 @@
         <v>24</v>
       </c>
       <c r="B5" t="n">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C5" t="n">
         <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="E5" t="n">
         <v>309</v>
       </c>
       <c r="F5" t="n">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G5" t="n">
         <v>175</v>
@@ -6418,13 +6418,13 @@
         <v>27</v>
       </c>
       <c r="B8" t="n">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C8" t="n">
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E8" t="n">
         <v>304</v>
@@ -6669,7 +6669,7 @@
         <v>25</v>
       </c>
       <c r="F13" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G13" t="n">
         <v>9</v>
@@ -7146,7 +7146,7 @@
         <v>8.460000000000001</v>
       </c>
       <c r="M2" t="n">
-        <v>925.63</v>
+        <v>879.5700000000001</v>
       </c>
       <c r="N2" t="n">
         <v>464.06</v>
@@ -7155,18 +7155,18 @@
         <v>20.69</v>
       </c>
       <c r="P2" t="n">
-        <v>74438.48</v>
+        <v>78774.74000000001</v>
       </c>
       <c r="Q2" t="s"/>
       <c r="R2" t="s"/>
       <c r="S2" t="n">
-        <v>988.99</v>
+        <v>2134.66</v>
       </c>
       <c r="T2" t="n">
         <v>179.07</v>
       </c>
       <c r="U2" t="n">
-        <v>90720.12</v>
+        <v>97759.88</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -7174,55 +7174,55 @@
         <v>22</v>
       </c>
       <c r="B3" t="n">
-        <v>9496.75</v>
+        <v>9552.440000000001</v>
       </c>
       <c r="C3" t="n">
         <v>42.5</v>
       </c>
       <c r="D3" t="n">
-        <v>16909.72</v>
+        <v>17056.75</v>
       </c>
       <c r="E3" t="n">
-        <v>10845.35</v>
+        <v>10938.18</v>
       </c>
       <c r="F3" t="n">
-        <v>17007.95</v>
+        <v>17148.28</v>
       </c>
       <c r="G3" t="n">
-        <v>3845.22</v>
+        <v>3877.56</v>
       </c>
       <c r="H3" t="n">
-        <v>10821.03</v>
+        <v>10860.69</v>
       </c>
       <c r="I3" t="n">
-        <v>9184.51</v>
+        <v>9226.629999999999</v>
       </c>
       <c r="J3" t="n">
-        <v>10945.65</v>
+        <v>11072.29</v>
       </c>
       <c r="K3" t="n">
-        <v>3322.31</v>
+        <v>3334.99</v>
       </c>
       <c r="L3" t="n">
-        <v>12020.99</v>
+        <v>12046.87</v>
       </c>
       <c r="M3" t="n">
-        <v>8377.49</v>
+        <v>8409.58</v>
       </c>
       <c r="N3" t="n">
-        <v>1876.13</v>
+        <v>1889.25</v>
       </c>
       <c r="O3" t="n">
-        <v>1988.52</v>
+        <v>1988.74</v>
       </c>
       <c r="P3" t="n">
-        <v>922.26</v>
+        <v>923.05</v>
       </c>
       <c r="Q3" t="n">
         <v>2471.26</v>
       </c>
       <c r="R3" t="n">
-        <v>2680.4</v>
+        <v>2687.38</v>
       </c>
       <c r="S3" t="n">
         <v>304.55</v>
@@ -7239,40 +7239,40 @@
         <v>23</v>
       </c>
       <c r="B4" t="n">
-        <v>4416.08</v>
+        <v>4415.94</v>
       </c>
       <c r="C4" t="n">
         <v>303.93</v>
       </c>
       <c r="D4" t="n">
-        <v>4399.61</v>
+        <v>4336.35</v>
       </c>
       <c r="E4" t="n">
         <v>2986.57</v>
       </c>
       <c r="F4" t="n">
-        <v>7904.83</v>
+        <v>7904.55</v>
       </c>
       <c r="G4" t="n">
-        <v>2809.11</v>
+        <v>2809.03</v>
       </c>
       <c r="H4" t="n">
-        <v>13007.94</v>
+        <v>13007.26</v>
       </c>
       <c r="I4" t="n">
-        <v>12788.22</v>
+        <v>12726.92</v>
       </c>
       <c r="J4" t="n">
-        <v>14346.1</v>
+        <v>14377.86</v>
       </c>
       <c r="K4" t="n">
-        <v>10244.91</v>
+        <v>10239.45</v>
       </c>
       <c r="L4" t="n">
-        <v>9214.01</v>
+        <v>9212.93</v>
       </c>
       <c r="M4" t="n">
-        <v>5045.02</v>
+        <v>5028.93</v>
       </c>
       <c r="N4" t="n">
         <v>3859.2</v>
@@ -7290,7 +7290,7 @@
         <v>645.88</v>
       </c>
       <c r="S4" t="n">
-        <v>240.09</v>
+        <v>239.82</v>
       </c>
       <c r="T4" t="n">
         <v>763.72</v>
@@ -7304,19 +7304,19 @@
         <v>24</v>
       </c>
       <c r="B5" t="n">
-        <v>925.09</v>
+        <v>916.84</v>
       </c>
       <c r="C5" t="n">
         <v>9.710000000000001</v>
       </c>
       <c r="D5" t="n">
-        <v>2775.86</v>
+        <v>2764.77</v>
       </c>
       <c r="E5" t="n">
         <v>1181.39</v>
       </c>
       <c r="F5" t="n">
-        <v>1628.85</v>
+        <v>1621.28</v>
       </c>
       <c r="G5" t="n">
         <v>579.86</v>
@@ -7325,7 +7325,7 @@
         <v>2109.81</v>
       </c>
       <c r="I5" t="n">
-        <v>2079.45</v>
+        <v>2077.83</v>
       </c>
       <c r="J5" t="n">
         <v>2205.81</v>
@@ -7337,7 +7337,7 @@
         <v>4340.21</v>
       </c>
       <c r="M5" t="n">
-        <v>7261.51</v>
+        <v>7251.17</v>
       </c>
       <c r="N5" t="n">
         <v>1535.81</v>
@@ -7405,7 +7405,7 @@
         <v>4031.46</v>
       </c>
       <c r="R6" t="n">
-        <v>8776.540000000001</v>
+        <v>8716.530000000001</v>
       </c>
       <c r="S6" t="s"/>
       <c r="T6" t="n">
@@ -7442,19 +7442,19 @@
         <v>2205.63</v>
       </c>
       <c r="J7" t="n">
-        <v>4644.65</v>
+        <v>4644.05</v>
       </c>
       <c r="K7" t="n">
         <v>1043.49</v>
       </c>
       <c r="L7" t="n">
-        <v>4943.76</v>
+        <v>4892.18</v>
       </c>
       <c r="M7" t="n">
-        <v>6814.14</v>
+        <v>6789.38</v>
       </c>
       <c r="N7" t="n">
-        <v>1883.66</v>
+        <v>1881.63</v>
       </c>
       <c r="O7" t="n">
         <v>1044.85</v>
@@ -7483,13 +7483,13 @@
         <v>27</v>
       </c>
       <c r="B8" t="n">
-        <v>865.9299999999999</v>
+        <v>862.66</v>
       </c>
       <c r="C8" t="n">
         <v>2.55</v>
       </c>
       <c r="D8" t="n">
-        <v>2871.3</v>
+        <v>2868.96</v>
       </c>
       <c r="E8" t="n">
         <v>1228.75</v>
@@ -7513,7 +7513,7 @@
         <v>673.36</v>
       </c>
       <c r="L8" t="n">
-        <v>2152.44</v>
+        <v>2144.91</v>
       </c>
       <c r="M8" t="n">
         <v>3532.07</v>
@@ -7571,7 +7571,7 @@
         <v>19.24</v>
       </c>
       <c r="K9" t="n">
-        <v>313.77</v>
+        <v>313.49</v>
       </c>
       <c r="L9" t="n">
         <v>186.06</v>
@@ -7603,7 +7603,7 @@
       </c>
       <c r="C10" t="s"/>
       <c r="D10" t="n">
-        <v>412.14</v>
+        <v>415.33</v>
       </c>
       <c r="E10" t="n">
         <v>343.34</v>
@@ -7615,10 +7615,10 @@
         <v>250.85</v>
       </c>
       <c r="H10" t="n">
-        <v>2617.57</v>
+        <v>2618</v>
       </c>
       <c r="I10" t="n">
-        <v>1183.15</v>
+        <v>1180.58</v>
       </c>
       <c r="J10" t="n">
         <v>2238.4</v>
@@ -7627,14 +7627,14 @@
         <v>1045</v>
       </c>
       <c r="L10" t="n">
-        <v>2749.17</v>
+        <v>2748.42</v>
       </c>
       <c r="M10" t="n">
-        <v>5102.4</v>
+        <v>5403.77</v>
       </c>
       <c r="N10" t="s"/>
       <c r="O10" t="n">
-        <v>351.51</v>
+        <v>347.54</v>
       </c>
       <c r="P10" t="s"/>
       <c r="Q10" t="s"/>
@@ -7665,13 +7665,13 @@
         <v>1163.36</v>
       </c>
       <c r="G11" t="n">
-        <v>339.39</v>
+        <v>345.71</v>
       </c>
       <c r="H11" t="n">
         <v>844.15</v>
       </c>
       <c r="I11" t="n">
-        <v>2175.19</v>
+        <v>2184.71</v>
       </c>
       <c r="J11" t="n">
         <v>1671.06</v>
@@ -7690,7 +7690,7 @@
       </c>
       <c r="O11" t="s"/>
       <c r="P11" t="n">
-        <v>661.15</v>
+        <v>710.24</v>
       </c>
       <c r="Q11" t="n">
         <v>59.67</v>
@@ -7701,7 +7701,7 @@
       <c r="S11" t="s"/>
       <c r="T11" t="s"/>
       <c r="U11" t="n">
-        <v>505.95</v>
+        <v>640.3099999999999</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -7766,7 +7766,7 @@
         <v>32</v>
       </c>
       <c r="B13" t="n">
-        <v>587.89</v>
+        <v>587.1900000000001</v>
       </c>
       <c r="C13" t="n">
         <v>2.42</v>
@@ -7775,10 +7775,10 @@
         <v>640.59</v>
       </c>
       <c r="E13" t="n">
-        <v>916.5</v>
+        <v>916.1900000000001</v>
       </c>
       <c r="F13" t="n">
-        <v>2025.98</v>
+        <v>2004.46</v>
       </c>
       <c r="G13" t="n">
         <v>542.91</v>
@@ -7799,10 +7799,10 @@
         <v>2295.97</v>
       </c>
       <c r="M13" t="n">
-        <v>3905.31</v>
+        <v>3903.49</v>
       </c>
       <c r="N13" t="n">
-        <v>554.27</v>
+        <v>552.54</v>
       </c>
       <c r="O13" t="s"/>
       <c r="P13" t="s"/>
@@ -7821,7 +7821,7 @@
         <v>33</v>
       </c>
       <c r="B14" t="n">
-        <v>520.1900000000001</v>
+        <v>520.15</v>
       </c>
       <c r="C14" t="n">
         <v>4.45</v>
@@ -7836,7 +7836,7 @@
         <v>528.9299999999999</v>
       </c>
       <c r="G14" t="n">
-        <v>527.05</v>
+        <v>526.95</v>
       </c>
       <c r="H14" t="n">
         <v>1366.42</v>
@@ -7851,7 +7851,7 @@
         <v>85.2</v>
       </c>
       <c r="L14" t="n">
-        <v>8525.49</v>
+        <v>8524.74</v>
       </c>
       <c r="M14" t="n">
         <v>1416.09</v>
@@ -7876,7 +7876,7 @@
         <v>34</v>
       </c>
       <c r="B15" t="n">
-        <v>393.07</v>
+        <v>393.01</v>
       </c>
       <c r="C15" t="n">
         <v>5.94</v>
@@ -7906,7 +7906,7 @@
         <v>400.29</v>
       </c>
       <c r="L15" t="n">
-        <v>450.72</v>
+        <v>450.71</v>
       </c>
       <c r="M15" t="n">
         <v>8152.84</v>
@@ -8057,7 +8057,7 @@
         <v>172.78</v>
       </c>
       <c r="J18" t="n">
-        <v>423.74</v>
+        <v>403.99</v>
       </c>
       <c r="K18" t="n">
         <v>264.06</v>
@@ -8082,7 +8082,7 @@
         <v>100.67</v>
       </c>
       <c r="S18" t="n">
-        <v>714.91</v>
+        <v>699.11</v>
       </c>
       <c r="T18" t="n">
         <v>350.56</v>
@@ -8147,7 +8147,7 @@
         <v>1.1</v>
       </c>
       <c r="S19" t="n">
-        <v>275.23</v>
+        <v>275.4</v>
       </c>
       <c r="T19" t="n">
         <v>199.56</v>
@@ -8313,25 +8313,25 @@
       <c r="J2" t="s"/>
       <c r="K2" t="s"/>
       <c r="L2" t="n">
-        <v>849.9400000000001</v>
+        <v>803.88</v>
       </c>
       <c r="M2" t="n">
         <v>464.06</v>
       </c>
       <c r="N2" t="s"/>
       <c r="O2" t="n">
-        <v>74438.48</v>
+        <v>78774.74000000001</v>
       </c>
       <c r="P2" t="s"/>
       <c r="Q2" t="s"/>
       <c r="R2" t="n">
-        <v>988.99</v>
+        <v>2134.66</v>
       </c>
       <c r="S2" t="n">
         <v>179.07</v>
       </c>
       <c r="T2" t="n">
-        <v>90720.12</v>
+        <v>97759.88</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -8339,52 +8339,52 @@
         <v>22</v>
       </c>
       <c r="B3" t="n">
-        <v>4011.04</v>
+        <v>4031.24</v>
       </c>
       <c r="C3" t="n">
-        <v>15323.32</v>
+        <v>15462.34</v>
       </c>
       <c r="D3" t="n">
-        <v>9838.68</v>
+        <v>9931.5</v>
       </c>
       <c r="E3" t="n">
-        <v>15401.44</v>
+        <v>15534.43</v>
       </c>
       <c r="F3" t="n">
-        <v>3478.4</v>
+        <v>3506.29</v>
       </c>
       <c r="G3" t="n">
-        <v>9320.32</v>
+        <v>9359.540000000001</v>
       </c>
       <c r="H3" t="n">
-        <v>6990.36</v>
+        <v>7021.5</v>
       </c>
       <c r="I3" t="n">
-        <v>9935.34</v>
+        <v>10061.94</v>
       </c>
       <c r="J3" t="n">
-        <v>3146.66</v>
+        <v>3159.09</v>
       </c>
       <c r="K3" t="n">
-        <v>9944.379999999999</v>
+        <v>9970.27</v>
       </c>
       <c r="L3" t="n">
-        <v>7677.72</v>
+        <v>7709.81</v>
       </c>
       <c r="M3" t="n">
-        <v>1412.52</v>
+        <v>1425.65</v>
       </c>
       <c r="N3" t="n">
-        <v>869.77</v>
+        <v>869.99</v>
       </c>
       <c r="O3" t="n">
-        <v>886</v>
+        <v>886.78</v>
       </c>
       <c r="P3" t="n">
         <v>2471.26</v>
       </c>
       <c r="Q3" t="n">
-        <v>2648.24</v>
+        <v>2655.22</v>
       </c>
       <c r="R3" t="n">
         <v>304.55</v>
@@ -8473,7 +8473,7 @@
         <v>185.52</v>
       </c>
       <c r="H5" t="n">
-        <v>348.59</v>
+        <v>346.97</v>
       </c>
       <c r="I5" t="n">
         <v>893.6900000000001</v>
@@ -8485,7 +8485,7 @@
         <v>3203.93</v>
       </c>
       <c r="L5" t="n">
-        <v>6543.65</v>
+        <v>6533.3</v>
       </c>
       <c r="M5" t="n">
         <v>1256.6</v>
@@ -8546,7 +8546,7 @@
         <v>4031.46</v>
       </c>
       <c r="Q6" t="n">
-        <v>8776.540000000001</v>
+        <v>8716.530000000001</v>
       </c>
       <c r="R6" t="s"/>
       <c r="S6" t="n">
@@ -8582,19 +8582,19 @@
         <v>1507.9</v>
       </c>
       <c r="I7" t="n">
-        <v>4446.42</v>
+        <v>4445.81</v>
       </c>
       <c r="J7" t="n">
         <v>916.58</v>
       </c>
       <c r="K7" t="n">
-        <v>4888.41</v>
+        <v>4836.83</v>
       </c>
       <c r="L7" t="n">
-        <v>6712.85</v>
+        <v>6688.09</v>
       </c>
       <c r="M7" t="n">
-        <v>1688.16</v>
+        <v>1686.13</v>
       </c>
       <c r="N7" t="n">
         <v>1044.85</v>
@@ -8650,7 +8650,7 @@
         <v>616.03</v>
       </c>
       <c r="K8" t="n">
-        <v>1981.77</v>
+        <v>1974.24</v>
       </c>
       <c r="L8" t="n">
         <v>3526.69</v>
@@ -8699,7 +8699,7 @@
         <v>19.24</v>
       </c>
       <c r="J9" t="n">
-        <v>313.77</v>
+        <v>313.49</v>
       </c>
       <c r="K9" t="n">
         <v>186.06</v>
@@ -8730,7 +8730,7 @@
         <v>11.77</v>
       </c>
       <c r="C10" t="n">
-        <v>73.06999999999999</v>
+        <v>76.27</v>
       </c>
       <c r="D10" t="n">
         <v>183.29</v>
@@ -8742,10 +8742,10 @@
         <v>228.36</v>
       </c>
       <c r="G10" t="n">
-        <v>2191.09</v>
+        <v>2191.51</v>
       </c>
       <c r="H10" t="n">
-        <v>1128.04</v>
+        <v>1125.46</v>
       </c>
       <c r="I10" t="n">
         <v>2202.12</v>
@@ -8754,14 +8754,14 @@
         <v>1004.75</v>
       </c>
       <c r="K10" t="n">
-        <v>2727.72</v>
+        <v>2726.97</v>
       </c>
       <c r="L10" t="n">
-        <v>5057.97</v>
+        <v>5359.34</v>
       </c>
       <c r="M10" t="s"/>
       <c r="N10" t="n">
-        <v>351.51</v>
+        <v>347.54</v>
       </c>
       <c r="O10" t="s"/>
       <c r="P10" t="s"/>
@@ -8791,13 +8791,13 @@
         <v>736.92</v>
       </c>
       <c r="F11" t="n">
-        <v>293.73</v>
+        <v>300.05</v>
       </c>
       <c r="G11" t="n">
         <v>696.2</v>
       </c>
       <c r="H11" t="n">
-        <v>1837.7</v>
+        <v>1847.21</v>
       </c>
       <c r="I11" t="n">
         <v>1522.78</v>
@@ -8816,7 +8816,7 @@
       </c>
       <c r="N11" t="s"/>
       <c r="O11" t="n">
-        <v>661.15</v>
+        <v>710.24</v>
       </c>
       <c r="P11" t="n">
         <v>59.67</v>
@@ -8827,7 +8827,7 @@
       <c r="R11" t="s"/>
       <c r="S11" t="s"/>
       <c r="T11" t="n">
-        <v>463.45</v>
+        <v>597.8099999999999</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -8889,16 +8889,16 @@
         <v>32</v>
       </c>
       <c r="B13" t="n">
-        <v>178.22</v>
+        <v>177.52</v>
       </c>
       <c r="C13" t="n">
         <v>297.64</v>
       </c>
       <c r="D13" t="n">
-        <v>604.73</v>
+        <v>604.4299999999999</v>
       </c>
       <c r="E13" t="n">
-        <v>1623.23</v>
+        <v>1623.21</v>
       </c>
       <c r="F13" t="n">
         <v>429.05</v>
@@ -8919,10 +8919,10 @@
         <v>2198.8</v>
       </c>
       <c r="L13" t="n">
-        <v>3767.56</v>
+        <v>3765.74</v>
       </c>
       <c r="M13" t="n">
-        <v>519.76</v>
+        <v>518.03</v>
       </c>
       <c r="N13" t="s"/>
       <c r="O13" t="s"/>
@@ -8968,7 +8968,7 @@
         <v>4.56</v>
       </c>
       <c r="K14" t="n">
-        <v>8171.26</v>
+        <v>8170.51</v>
       </c>
       <c r="L14" t="n">
         <v>1394.84</v>
@@ -9148,7 +9148,7 @@
         <v>11.59</v>
       </c>
       <c r="I18" t="n">
-        <v>324.1</v>
+        <v>304.34</v>
       </c>
       <c r="J18" t="n">
         <v>256.58</v>
@@ -9173,7 +9173,7 @@
         <v>100.67</v>
       </c>
       <c r="R18" t="n">
-        <v>714.91</v>
+        <v>699.11</v>
       </c>
       <c r="S18" t="n">
         <v>350.56</v>
@@ -9229,7 +9229,7 @@
         <v>1.1</v>
       </c>
       <c r="R19" t="n">
-        <v>273.82</v>
+        <v>273.99</v>
       </c>
       <c r="S19" t="n">
         <v>193.12</v>
@@ -9420,34 +9420,34 @@
         <v>22</v>
       </c>
       <c r="B3" t="n">
-        <v>5485.7</v>
+        <v>5521.2</v>
       </c>
       <c r="C3" t="n">
         <v>42.5</v>
       </c>
       <c r="D3" t="n">
-        <v>1586.41</v>
+        <v>1594.4</v>
       </c>
       <c r="E3" t="n">
         <v>1006.67</v>
       </c>
       <c r="F3" t="n">
-        <v>1606.5</v>
+        <v>1613.85</v>
       </c>
       <c r="G3" t="n">
-        <v>366.83</v>
+        <v>371.26</v>
       </c>
       <c r="H3" t="n">
-        <v>1500.71</v>
+        <v>1501.14</v>
       </c>
       <c r="I3" t="n">
-        <v>2194.15</v>
+        <v>2205.13</v>
       </c>
       <c r="J3" t="n">
-        <v>1010.31</v>
+        <v>1010.35</v>
       </c>
       <c r="K3" t="n">
-        <v>175.66</v>
+        <v>175.9</v>
       </c>
       <c r="L3" t="n">
         <v>2076.61</v>
@@ -9479,40 +9479,40 @@
         <v>23</v>
       </c>
       <c r="B4" t="n">
-        <v>4416.08</v>
+        <v>4415.94</v>
       </c>
       <c r="C4" t="n">
         <v>303.93</v>
       </c>
       <c r="D4" t="n">
-        <v>4256.12</v>
+        <v>4192.87</v>
       </c>
       <c r="E4" t="n">
         <v>2881.45</v>
       </c>
       <c r="F4" t="n">
-        <v>7897.87</v>
+        <v>7897.6</v>
       </c>
       <c r="G4" t="n">
-        <v>2804.67</v>
+        <v>2804.58</v>
       </c>
       <c r="H4" t="n">
-        <v>12809.96</v>
+        <v>12809.28</v>
       </c>
       <c r="I4" t="n">
-        <v>12689.43</v>
+        <v>12628.13</v>
       </c>
       <c r="J4" t="n">
-        <v>13334.59</v>
+        <v>13366.35</v>
       </c>
       <c r="K4" t="n">
-        <v>4442.48</v>
+        <v>4437.02</v>
       </c>
       <c r="L4" t="n">
-        <v>7551.37</v>
+        <v>7550.29</v>
       </c>
       <c r="M4" t="n">
-        <v>4437.04</v>
+        <v>4420.95</v>
       </c>
       <c r="N4" t="n">
         <v>2317.82</v>
@@ -9530,7 +9530,7 @@
         <v>79.26000000000001</v>
       </c>
       <c r="S4" t="n">
-        <v>240.09</v>
+        <v>239.82</v>
       </c>
       <c r="T4" t="n">
         <v>599.1900000000001</v>
@@ -9544,19 +9544,19 @@
         <v>24</v>
       </c>
       <c r="B5" t="n">
-        <v>925.09</v>
+        <v>916.84</v>
       </c>
       <c r="C5" t="n">
         <v>9.710000000000001</v>
       </c>
       <c r="D5" t="n">
-        <v>2733.41</v>
+        <v>2722.32</v>
       </c>
       <c r="E5" t="n">
         <v>1171.87</v>
       </c>
       <c r="F5" t="n">
-        <v>1574.97</v>
+        <v>1567.4</v>
       </c>
       <c r="G5" t="n">
         <v>570.6799999999999</v>
@@ -9693,13 +9693,13 @@
         <v>27</v>
       </c>
       <c r="B8" t="n">
-        <v>848.75</v>
+        <v>845.49</v>
       </c>
       <c r="C8" t="n">
         <v>2.55</v>
       </c>
       <c r="D8" t="n">
-        <v>2829.35</v>
+        <v>2827.02</v>
       </c>
       <c r="E8" t="n">
         <v>949.58</v>
@@ -9944,7 +9944,7 @@
         <v>311.76</v>
       </c>
       <c r="F13" t="n">
-        <v>402.75</v>
+        <v>381.25</v>
       </c>
       <c r="G13" t="n">
         <v>113.86</v>
@@ -9981,7 +9981,7 @@
         <v>33</v>
       </c>
       <c r="B14" t="n">
-        <v>397.82</v>
+        <v>397.78</v>
       </c>
       <c r="C14" t="n">
         <v>4.45</v>
@@ -9996,7 +9996,7 @@
         <v>182.37</v>
       </c>
       <c r="G14" t="n">
-        <v>141.47</v>
+        <v>141.38</v>
       </c>
       <c r="H14" t="n">
         <v>470.15</v>
@@ -10030,7 +10030,7 @@
         <v>34</v>
       </c>
       <c r="B15" t="n">
-        <v>366.23</v>
+        <v>366.18</v>
       </c>
       <c r="C15" t="n">
         <v>5.94</v>
@@ -10060,7 +10060,7 @@
         <v>24.41</v>
       </c>
       <c r="L15" t="n">
-        <v>89.40000000000001</v>
+        <v>89.39</v>
       </c>
       <c r="M15" t="s"/>
       <c r="N15" t="s"/>

</xml_diff>